<commit_message>
Solicitudes gráficas y audio
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/SolicitudGrafica_LE_08_01_REC310.xlsx
+++ b/fuentes/contenidos/grado08/guion01/SolicitudGrafica_LE_08_01_REC310.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luz Amparo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luz Amparo\Documents\GitHub\Lenguaje\fuentes\contenidos\grado08\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="hX79YNGfHMUCcosWMoH0GQuhNo2gkebFrfW3do2TOcvwqaujU9m0uwOL5UkRtWEspAy/ISD2JB8+jf057W9mVA==" workbookSaltValue="uRz/CDpmZ5ecKheoN1C0Jw==" workbookSpinCount="100000" lockStructure="1"/>
@@ -599,7 +599,7 @@
     <t>Fotografía</t>
   </si>
   <si>
-    <t>LE_08_01_REC320</t>
+    <t>LE_08_01_REC310</t>
   </si>
 </sst>
 </file>
@@ -2966,7 +2966,7 @@
       </c>
       <c r="F10" s="13" t="str">
         <f t="shared" ref="F10" ca="1" si="1">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I10="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>LE_08_01_REC320_IMG01.jpg</v>
+        <v>LE_08_01_REC310_IMG01.jpg</v>
       </c>
       <c r="G10" s="13" t="str">
         <f ca="1">IF($F10&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E10,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3007,7 +3007,7 @@
       </c>
       <c r="F11" s="13" t="str">
         <f t="shared" ref="F11:F74" ca="1" si="4">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>LE_08_01_REC320_IMG02.jpg</v>
+        <v>LE_08_01_REC310_IMG02.jpg</v>
       </c>
       <c r="G11" s="13" t="str">
         <f ca="1">IF($F11&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E11,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3048,7 +3048,7 @@
       </c>
       <c r="F12" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>LE_08_01_REC320_IMG03.jpg</v>
+        <v>LE_08_01_REC310_IMG03.jpg</v>
       </c>
       <c r="G12" s="13" t="str">
         <f ca="1">IF($F12&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E12,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3089,7 +3089,7 @@
       </c>
       <c r="F13" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>LE_08_01_REC320_IMG04.jpg</v>
+        <v>LE_08_01_REC310_IMG04.jpg</v>
       </c>
       <c r="G13" s="13" t="str">
         <f ca="1">IF($F13&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>

</xml_diff>